<commit_message>
Análisis de datos con Power Bi
proyecto para análisis de datos.
</commit_message>
<xml_diff>
--- a/salida/archivos-de-trabajo/sismos2.xlsx
+++ b/salida/archivos-de-trabajo/sismos2.xlsx
@@ -715,10 +715,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,6 +732,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -775,10 +784,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -787,8 +797,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1092,7 +1104,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1150,7 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
@@ -1161,7 +1173,7 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
@@ -1184,7 +1196,7 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
@@ -1207,7 +1219,7 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
@@ -1230,7 +1242,7 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
@@ -1253,7 +1265,7 @@
       <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E7" t="s">
@@ -1276,7 +1288,7 @@
       <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E8" t="s">
@@ -1299,7 +1311,7 @@
       <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E9" t="s">
@@ -1322,7 +1334,7 @@
       <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E10" t="s">
@@ -1345,7 +1357,7 @@
       <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E11" t="s">
@@ -1368,7 +1380,7 @@
       <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E12" t="s">
@@ -1391,7 +1403,7 @@
       <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E13" t="s">
@@ -1414,7 +1426,7 @@
       <c r="C14" t="s">
         <v>47</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
@@ -1437,7 +1449,7 @@
       <c r="C15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E15" t="s">
@@ -1460,7 +1472,7 @@
       <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E16" t="s">
@@ -1483,7 +1495,7 @@
       <c r="C17" t="s">
         <v>57</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
@@ -1506,7 +1518,7 @@
       <c r="C18" t="s">
         <v>59</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E18" t="s">
@@ -1529,7 +1541,7 @@
       <c r="C19" t="s">
         <v>62</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E19" t="s">
@@ -1552,7 +1564,7 @@
       <c r="C20" t="s">
         <v>65</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
@@ -1575,7 +1587,7 @@
       <c r="C21" t="s">
         <v>68</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E21" t="s">
@@ -1598,7 +1610,7 @@
       <c r="C22" t="s">
         <v>71</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E22" t="s">
@@ -1621,7 +1633,7 @@
       <c r="C23" t="s">
         <v>74</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
@@ -1644,7 +1656,7 @@
       <c r="C24" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E24" t="s">
@@ -1667,7 +1679,7 @@
       <c r="C25" t="s">
         <v>80</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E25" t="s">
@@ -1690,7 +1702,7 @@
       <c r="C26" t="s">
         <v>71</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="4" t="s">
         <v>83</v>
       </c>
       <c r="E26" t="s">
@@ -1713,7 +1725,7 @@
       <c r="C27" t="s">
         <v>86</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E27" t="s">
@@ -1736,7 +1748,7 @@
       <c r="C28" t="s">
         <v>89</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E28" t="s">
@@ -1759,7 +1771,7 @@
       <c r="C29" t="s">
         <v>92</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E29" t="s">
@@ -1782,7 +1794,7 @@
       <c r="C30" t="s">
         <v>94</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E30" t="s">
@@ -1805,7 +1817,7 @@
       <c r="C31" t="s">
         <v>97</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E31" t="s">
@@ -1828,7 +1840,7 @@
       <c r="C32" t="s">
         <v>100</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E32" t="s">
@@ -1851,7 +1863,7 @@
       <c r="C33" t="s">
         <v>103</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E33" t="s">
@@ -1874,7 +1886,7 @@
       <c r="C34" t="s">
         <v>106</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E34" t="s">
@@ -1897,7 +1909,7 @@
       <c r="C35" t="s">
         <v>109</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E35" t="s">
@@ -1920,7 +1932,7 @@
       <c r="C36" t="s">
         <v>111</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E36" t="s">
@@ -1943,7 +1955,7 @@
       <c r="C37" t="s">
         <v>113</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E37" t="s">
@@ -1966,7 +1978,7 @@
       <c r="C38" t="s">
         <v>115</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E38" t="s">
@@ -1989,7 +2001,7 @@
       <c r="C39" t="s">
         <v>118</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E39" t="s">
@@ -2012,7 +2024,7 @@
       <c r="C40" t="s">
         <v>120</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E40" t="s">
@@ -2035,7 +2047,7 @@
       <c r="C41" t="s">
         <v>123</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E41" t="s">
@@ -2058,7 +2070,7 @@
       <c r="C42" t="s">
         <v>126</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E42" t="s">
@@ -2081,7 +2093,7 @@
       <c r="C43" t="s">
         <v>129</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E43" t="s">
@@ -2104,7 +2116,7 @@
       <c r="C44" t="s">
         <v>131</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E44" t="s">
@@ -2127,7 +2139,7 @@
       <c r="C45" t="s">
         <v>134</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E45" t="s">
@@ -2150,7 +2162,7 @@
       <c r="C46" t="s">
         <v>137</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E46" t="s">
@@ -2173,7 +2185,7 @@
       <c r="C47" t="s">
         <v>139</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="4" t="s">
         <v>140</v>
       </c>
       <c r="E47" t="s">
@@ -2196,7 +2208,7 @@
       <c r="C48" t="s">
         <v>142</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E48" t="s">
@@ -2219,7 +2231,7 @@
       <c r="C49" t="s">
         <v>145</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E49" t="s">
@@ -2242,7 +2254,7 @@
       <c r="C50" t="s">
         <v>148</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E50" t="s">
@@ -2265,7 +2277,7 @@
       <c r="C51" t="s">
         <v>150</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="4" t="s">
         <v>151</v>
       </c>
       <c r="E51" t="s">
@@ -2288,7 +2300,7 @@
       <c r="C52" t="s">
         <v>153</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="4" t="s">
         <v>154</v>
       </c>
       <c r="E52" t="s">
@@ -2311,7 +2323,7 @@
       <c r="C53" t="s">
         <v>157</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E53" t="s">
@@ -2334,7 +2346,7 @@
       <c r="C54" t="s">
         <v>159</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E54" t="s">
@@ -2357,7 +2369,7 @@
       <c r="C55" t="s">
         <v>161</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E55" t="s">
@@ -2380,7 +2392,7 @@
       <c r="C56" t="s">
         <v>163</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E56" t="s">
@@ -2403,7 +2415,7 @@
       <c r="C57" t="s">
         <v>165</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E57" t="s">
@@ -2426,7 +2438,7 @@
       <c r="C58" t="s">
         <v>168</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E58" t="s">
@@ -2449,7 +2461,7 @@
       <c r="C59" t="s">
         <v>171</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E59" t="s">
@@ -2472,7 +2484,7 @@
       <c r="C60" t="s">
         <v>174</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E60" t="s">
@@ -2495,7 +2507,7 @@
       <c r="C61" t="s">
         <v>176</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E61" t="s">
@@ -2511,5 +2523,6 @@
   </sheetData>
   <autoFilter ref="A1:G61"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>